<commit_message>
Fixed some smal issue
</commit_message>
<xml_diff>
--- a/documents/test-case.xlsx
+++ b/documents/test-case.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cnpm\soen-bus\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test case tìm xe buýt (đúng)" sheetId="1" r:id="rId1"/>
+    <sheet name="Test case tìm xe buýt (sai)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>QA Tester’s Log</t>
   </si>
@@ -95,10 +96,19 @@
     <t>Nhập được</t>
   </si>
   <si>
-    <t>Khi vừa nhập xong hệ thống tự động tìm kiếm tuyến xe buýt</t>
-  </si>
-  <si>
-    <t>hiển thị tuyến xe buýt tương ứng</t>
+    <t>Nhấn vào "find route"</t>
+  </si>
+  <si>
+    <t>hiển thị địa chỉ đầy đủ của 2 điểm, dồng thời hiển thị tuyến xe buýt và các thông tin liên quan.</t>
+  </si>
+  <si>
+    <t>Địa chỉ đến = dh</t>
+  </si>
+  <si>
+    <t>Địa chỉ đi = q</t>
+  </si>
+  <si>
+    <t>hiển thị chữ đỏ thông báo</t>
   </si>
 </sst>
 </file>
@@ -244,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -283,7 +293,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -292,9 +337,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -315,36 +357,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,17 +647,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -663,29 +682,29 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="33">
+      <c r="E3" s="18"/>
+      <c r="F3" s="20">
         <v>44325</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="35" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="35"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -704,94 +723,94 @@
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="10"/>
       <c r="F7" s="9">
         <v>2</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>3</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="10"/>
       <c r="F8" s="9">
         <v>3</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>4</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="10"/>
       <c r="F9" s="9">
         <v>4</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -837,165 +856,177 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="19" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="19" t="s">
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>1</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="15" t="s">
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="15" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="17"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>3</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="36"/>
+      <c r="F17" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="15" t="s">
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="17"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>4</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="17"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="B9:D9"/>
@@ -1005,6 +1036,346 @@
     <mergeCell ref="D13:E14"/>
     <mergeCell ref="F13:H14"/>
     <mergeCell ref="I13:K14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20">
+        <v>44325</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9">
+        <v>3</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9">
+        <v>4</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="27"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>3</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="F17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:K17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:H15"/>
@@ -1013,22 +1384,27 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:H14"/>
+    <mergeCell ref="I13:K14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>